<commit_message>
Refactored grid access, removed grid API
</commit_message>
<xml_diff>
--- a/files/Grids.xlsx
+++ b/files/Grids.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\git\sudoku\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3C121D-5E48-4CA9-9364-8A3D4D002745}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2420933E-DA6C-47EA-8157-FA8BA4394176}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-435" yWindow="-18120" windowWidth="29040" windowHeight="17640" xr2:uid="{DF23C0EB-D369-46C5-B273-920E95169029}"/>
+    <workbookView xWindow="5002" yWindow="1620" windowWidth="15271" windowHeight="11310" xr2:uid="{DF23C0EB-D369-46C5-B273-920E95169029}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Indices" sheetId="1" r:id="rId1"/>
+    <sheet name="Example" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -212,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -266,6 +267,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -582,334 +610,750 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA76EE9-AE6D-4FBF-9BA1-EE411859C0F4}">
-  <dimension ref="B1:K11"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.3984375" customWidth="1"/>
-    <col min="2" max="11" width="5.59765625" customWidth="1"/>
+    <col min="1" max="10" width="5.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1">
+    <row r="1" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
+      <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="E2" s="1">
+      <c r="D1" s="1">
         <v>3</v>
       </c>
-      <c r="F2" s="1">
+      <c r="E1" s="1">
         <v>4</v>
       </c>
-      <c r="G2" s="1">
+      <c r="F1" s="1">
         <v>5</v>
       </c>
-      <c r="H2" s="1">
+      <c r="G1" s="1">
         <v>6</v>
       </c>
-      <c r="I2" s="1">
+      <c r="H1" s="1">
         <v>7</v>
       </c>
-      <c r="J2" s="1">
+      <c r="I1" s="1">
         <v>8</v>
       </c>
-      <c r="K2" s="1">
+      <c r="J1" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="1">
+    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="11">
+      <c r="B2" s="19">
+        <f>(($A2-1)*9)+B$1-1</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="20">
+        <f t="shared" ref="C2:J10" si="0">(($A2-1)*9)+C$1-1</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E2" s="19">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F2" s="20">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G2" s="21">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D3" s="3">
+      <c r="H2" s="19">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I2" s="20">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J2" s="21">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="22">
+        <f t="shared" ref="B3:B10" si="1">(($A3-1)*9)+B$1-1</f>
         <v>9</v>
       </c>
-      <c r="E3" s="12">
+      <c r="C3" s="23">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D3" s="24">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E3" s="22">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F3" s="23">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G3" s="24">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="H3" s="22">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="I3" s="23">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="J3" s="24">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="25">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="C4" s="26">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D4" s="27">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E4" s="25">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="F4" s="26">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G4" s="27">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="H4" s="25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="I4" s="26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="J4" s="27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="19">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="C5" s="20">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D5" s="21">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="E5" s="19">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="F5" s="20">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="G5" s="21">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="H5" s="19">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="I5" s="20">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="J5" s="21">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="22">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="C6" s="23">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D6" s="24">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="E6" s="22">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="F6" s="23">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="G6" s="24">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="H6" s="22">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="I6" s="23">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="J6" s="24">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="25">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="C7" s="26">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D7" s="27">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="E7" s="25">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="F7" s="26">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="G7" s="27">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="H7" s="25">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="I7" s="26">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="J7" s="27">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="19">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="C8" s="20">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="D8" s="21">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="E8" s="19">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="F8" s="20">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="G8" s="21">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="H8" s="19">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="I8" s="20">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="J8" s="21">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="22">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="C9" s="23">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="D9" s="24">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="E9" s="22">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="F9" s="23">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="G9" s="24">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="H9" s="22">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="I9" s="23">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="J9" s="24">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="25">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="C10" s="26">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="D10" s="27">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="E10" s="25">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F10" s="26">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="G10" s="27">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="H10" s="25">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="I10" s="26">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="J10" s="27">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D3B3D7-E5AF-4286-8CBC-1519FFF705A7}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="10" width="5.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="2">
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
         <v>8</v>
       </c>
-      <c r="G3" s="13">
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3">
+        <v>9</v>
+      </c>
+      <c r="D2" s="12">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>8</v>
+      </c>
+      <c r="F2" s="13">
         <v>3</v>
       </c>
-      <c r="H3" s="4">
+      <c r="G2" s="4">
         <v>2</v>
       </c>
-      <c r="I3" s="2">
+      <c r="H2" s="2">
         <v>4</v>
       </c>
-      <c r="J3" s="13">
+      <c r="I2" s="13">
         <v>6</v>
       </c>
-      <c r="K3" s="4">
+      <c r="J2" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1">
+    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="5">
+      <c r="B3" s="5">
         <v>8</v>
       </c>
-      <c r="D4" s="6">
+      <c r="C3" s="6">
         <v>3</v>
       </c>
-      <c r="E4" s="7">
+      <c r="D3" s="7">
         <v>6</v>
       </c>
-      <c r="F4" s="15">
+      <c r="E3" s="15">
         <v>4</v>
       </c>
-      <c r="G4" s="6">
+      <c r="F3" s="6">
         <v>1</v>
       </c>
-      <c r="H4" s="7">
+      <c r="G3" s="7">
         <v>7</v>
       </c>
-      <c r="I4" s="15">
+      <c r="H3" s="15">
         <v>2</v>
       </c>
-      <c r="J4" s="6">
+      <c r="I3" s="6">
         <v>9</v>
       </c>
-      <c r="K4" s="7">
+      <c r="J3" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="1">
+    <row r="4" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="16">
+      <c r="B4" s="16">
         <v>7</v>
       </c>
-      <c r="D5" s="9">
+      <c r="C4" s="9">
         <v>4</v>
       </c>
-      <c r="E5" s="10">
+      <c r="D4" s="10">
         <v>2</v>
       </c>
-      <c r="F5" s="8">
+      <c r="E4" s="8">
         <v>5</v>
       </c>
-      <c r="G5" s="9">
+      <c r="F4" s="9">
         <v>6</v>
       </c>
-      <c r="H5" s="10">
+      <c r="G4" s="10">
         <v>9</v>
       </c>
-      <c r="I5" s="8">
+      <c r="H4" s="8">
         <v>1</v>
       </c>
-      <c r="J5" s="9">
+      <c r="I4" s="9">
         <v>8</v>
       </c>
-      <c r="K5" s="10">
+      <c r="J4" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="1">
+    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="2">
+      <c r="B5" s="2">
         <v>9</v>
       </c>
-      <c r="D6" s="13">
+      <c r="C5" s="13">
         <v>2</v>
       </c>
-      <c r="E6" s="12">
+      <c r="D5" s="12">
         <v>8</v>
       </c>
-      <c r="F6" s="2">
+      <c r="E5" s="2">
         <v>3</v>
       </c>
-      <c r="G6" s="3">
+      <c r="F5" s="3">
         <v>5</v>
       </c>
-      <c r="H6" s="4">
+      <c r="G5" s="4">
         <v>1</v>
       </c>
-      <c r="I6" s="2">
+      <c r="H5" s="2">
         <v>7</v>
       </c>
-      <c r="J6" s="3">
+      <c r="I5" s="3">
         <v>4</v>
       </c>
-      <c r="K6" s="4">
+      <c r="J5" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="1">
+    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="C7" s="5">
+      <c r="B6" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="6">
+      <c r="C6" s="6">
         <v>5</v>
       </c>
-      <c r="E7" s="7">
+      <c r="D6" s="7">
         <v>3</v>
       </c>
-      <c r="F7" s="5">
+      <c r="E6" s="5">
         <v>6</v>
       </c>
-      <c r="G7" s="17">
+      <c r="F6" s="17">
         <v>7</v>
       </c>
-      <c r="H7" s="7">
+      <c r="G6" s="7">
         <v>8</v>
       </c>
-      <c r="I7" s="5">
+      <c r="H6" s="5">
         <v>9</v>
       </c>
-      <c r="J7" s="6">
+      <c r="I6" s="6">
         <v>2</v>
       </c>
-      <c r="K7" s="14">
+      <c r="J6" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="1">
+    <row r="7" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="C8" s="8">
+      <c r="B7" s="8">
         <v>6</v>
       </c>
-      <c r="D8" s="9">
+      <c r="C7" s="9">
         <v>1</v>
       </c>
-      <c r="E8" s="10">
+      <c r="D7" s="10">
         <v>7</v>
       </c>
-      <c r="F8" s="8">
+      <c r="E7" s="8">
         <v>9</v>
       </c>
-      <c r="G8" s="9">
+      <c r="F7" s="9">
         <v>2</v>
       </c>
-      <c r="H8" s="10">
+      <c r="G7" s="10">
         <v>4</v>
       </c>
-      <c r="I8" s="8">
+      <c r="H7" s="8">
         <v>5</v>
       </c>
-      <c r="J8" s="18">
+      <c r="I7" s="18">
         <v>3</v>
       </c>
-      <c r="K8" s="10">
+      <c r="J7" s="10">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="1">
+    <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="C9" s="11">
+      <c r="B8" s="11">
         <v>1</v>
       </c>
-      <c r="D9" s="13">
+      <c r="C8" s="13">
         <v>6</v>
       </c>
-      <c r="E9" s="4">
+      <c r="D8" s="4">
         <v>4</v>
       </c>
-      <c r="F9" s="11">
+      <c r="E8" s="11">
         <v>2</v>
       </c>
-      <c r="G9" s="3">
+      <c r="F8" s="3">
         <v>8</v>
       </c>
-      <c r="H9" s="4">
+      <c r="G8" s="4">
         <v>5</v>
       </c>
-      <c r="I9" s="2">
+      <c r="H8" s="2">
         <v>3</v>
       </c>
-      <c r="J9" s="3">
+      <c r="I8" s="3">
         <v>7</v>
       </c>
-      <c r="K9" s="4">
+      <c r="J8" s="4">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="1">
+    <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="C10" s="5">
+      <c r="B9" s="5">
         <v>2</v>
       </c>
-      <c r="D10" s="6">
+      <c r="C9" s="6">
         <v>8</v>
       </c>
-      <c r="E10" s="7">
+      <c r="D9" s="7">
         <v>5</v>
       </c>
-      <c r="F10" s="5">
+      <c r="E9" s="5">
         <v>7</v>
       </c>
-      <c r="G10" s="6">
+      <c r="F9" s="6">
         <v>9</v>
       </c>
-      <c r="H10" s="7">
+      <c r="G9" s="7">
         <v>3</v>
       </c>
-      <c r="I10" s="5">
+      <c r="H9" s="5">
         <v>6</v>
       </c>
-      <c r="J10" s="6">
+      <c r="I9" s="6">
         <v>1</v>
       </c>
-      <c r="K10" s="14">
+      <c r="J9" s="14">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="1">
+    <row r="10" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="C11" s="8">
+      <c r="B10" s="8">
         <v>3</v>
       </c>
-      <c r="D11" s="9">
+      <c r="C10" s="9">
         <v>7</v>
       </c>
-      <c r="E11" s="10">
+      <c r="D10" s="10">
         <v>9</v>
       </c>
-      <c r="F11" s="8">
+      <c r="E10" s="8">
         <v>1</v>
       </c>
-      <c r="G11" s="9">
+      <c r="F10" s="9">
         <v>4</v>
       </c>
-      <c r="H11" s="10">
+      <c r="G10" s="10">
         <v>6</v>
       </c>
-      <c r="I11" s="16">
+      <c r="H10" s="16">
         <v>8</v>
       </c>
-      <c r="J11" s="9">
+      <c r="I10" s="9">
         <v>5</v>
       </c>
-      <c r="K11" s="10">
+      <c r="J10" s="10">
         <v>2</v>
       </c>
     </row>

</xml_diff>